<commit_message>
Added 4 new tile for Door controlled by switch
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonholmes/projects/RogueBoy_Pokitto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scote/Downloads/RogueBoy_Pokitto-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5409CC96-DE2D-EB4D-BDB2-6DF318BF4952}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4853454E-D4B7-664E-83C1-EDA00107439D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="480" windowWidth="51200" windowHeight="26820" xr2:uid="{14B29CA5-D18D-E94B-95B9-2B8B7C34E42E}"/>
+    <workbookView xWindow="2380" yWindow="6560" windowWidth="51200" windowHeight="26820" xr2:uid="{14B29CA5-D18D-E94B-95B9-2B8B7C34E42E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>NewStraightRHS</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>NewEndTBL</t>
+  </si>
+  <si>
+    <t>NewSwitchDoorLHS</t>
+  </si>
+  <si>
+    <t>NewSwitchDoorRHS</t>
+  </si>
+  <si>
+    <t>NewSwitchDoorTOP</t>
+  </si>
+  <si>
+    <t>NewSwitchDoorBOT</t>
   </si>
 </sst>
 </file>
@@ -1568,6 +1580,182 @@
         <a:xfrm>
           <a:off x="4167925" y="484925"/>
           <a:ext cx="101600" cy="101600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53554</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>22953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>160663</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>130062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1431A23-288A-404B-947E-5C28D74CF61D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4307289" y="635001"/>
+          <a:ext cx="107109" cy="107109"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53554</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>11482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>164488</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>122416</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDB6A041-3869-C745-A095-A167125F8FBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4307289" y="776542"/>
+          <a:ext cx="110934" cy="110934"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53554</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15302</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>172138</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{299D279C-BBDE-B346-9ABC-6CF603998DFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4307289" y="933374"/>
+          <a:ext cx="118584" cy="118584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53554</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>26777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>179789</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>153012</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{395C2217-9F93-424B-9273-591724D2BD65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4307289" y="1097861"/>
+          <a:ext cx="126235" cy="126235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1882,7 +2070,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="332" zoomScaleNormal="332" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2025,6 +2213,12 @@
       <c r="I5" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="J5" s="1">
+        <v>57</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
@@ -2045,6 +2239,12 @@
       <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="J6" s="1">
+        <v>58</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
@@ -2065,6 +2265,12 @@
       <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="J7" s="1">
+        <v>59</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
@@ -2084,6 +2290,12 @@
       </c>
       <c r="I8" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="J8" s="1">
+        <v>60</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>